<commit_message>
Agregado placa todo en uno
</commit_message>
<xml_diff>
--- a/other stuff/Precio.xlsx
+++ b/other stuff/Precio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alumno\Desktop\Proyecto\other stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Jeremias\Escritorio\Trabajos colegio\Proyecto final\other stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5D0DDC1-20B6-41CD-A734-DC23F6F1F8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808CC818-31B3-4B86-90E6-0B306E381DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{FE0F1B0A-B804-4440-98A7-4736C99B4B35}"/>
+    <workbookView xWindow="-22905" yWindow="1335" windowWidth="21600" windowHeight="11295" xr2:uid="{FE0F1B0A-B804-4440-98A7-4736C99B4B35}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -57,9 +56,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;\ #,##0.00;[Red]\-&quot;$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;\ #,##0.00;[Red]\-&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -167,7 +166,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -180,29 +179,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -522,7 +521,7 @@
   <dimension ref="C2:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,113 +544,115 @@
       </c>
     </row>
     <row r="4" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <v>600</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="7">
         <v>30</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="7">
         <v>315</v>
       </c>
     </row>
     <row r="5" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="8">
+      <c r="C5" s="6">
         <v>50</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="7">
         <v>414</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="7">
         <v>450</v>
       </c>
     </row>
     <row r="6" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="8">
+      <c r="C6" s="6">
         <v>200</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="7">
         <v>60</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="7">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="10">
+      <c r="C7" s="8">
         <v>650</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="7">
         <v>1000</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="7">
         <v>3907</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="10"/>
-      <c r="D8" s="9">
+      <c r="C8" s="8">
+        <v>2600</v>
+      </c>
+      <c r="D8" s="7">
         <v>2618</v>
       </c>
-      <c r="E8" s="11"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="10"/>
-      <c r="D9" s="9">
+      <c r="C9" s="8"/>
+      <c r="D9" s="7">
         <v>311</v>
       </c>
-      <c r="E9" s="11"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="10"/>
-      <c r="D10" s="11">
+      <c r="C10" s="8"/>
+      <c r="D10" s="9">
         <v>440</v>
       </c>
-      <c r="E10" s="11"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="10"/>
-      <c r="D11" s="11">
+      <c r="C11" s="8"/>
+      <c r="D11" s="9">
         <v>830</v>
       </c>
-      <c r="E11" s="11"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="10"/>
-      <c r="D12" s="11">
+      <c r="C12" s="8"/>
+      <c r="D12" s="9">
         <v>450</v>
       </c>
-      <c r="E12" s="11"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="10"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="10"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="4">
         <f>SUM(C4:C17)</f>
-        <v>1500</v>
+        <v>4100</v>
       </c>
       <c r="D18" s="5">
         <f>SUM(D4:D17)</f>
@@ -666,21 +667,21 @@
       <c r="C19" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="10">
         <f>SUM(C18:E18)</f>
-        <v>12345</v>
-      </c>
-      <c r="E19" s="7"/>
+        <v>14945</v>
+      </c>
+      <c r="E19" s="11"/>
     </row>
     <row r="20" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="10">
         <f>(D19/3)</f>
-        <v>4115</v>
-      </c>
-      <c r="E20" s="7"/>
+        <v>4981.666666666667</v>
+      </c>
+      <c r="E20" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>